<commit_message>
Tornado plot tutorial finished.
</commit_message>
<xml_diff>
--- a/Files/TornadoPlotExampleData.xlsx
+++ b/Files/TornadoPlotExampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spauliuk\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spauliuk\FILES\ARBEIT\Software\IPython\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
         <v>-1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>-0.5</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -475,7 +475,7 @@
         <v>-1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -606,7 +606,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-2</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -650,13 +650,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>-0.5</v>
+        <v>-4</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D11">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -717,7 +717,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -784,10 +784,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C17">
-        <v>1.5</v>
+        <v>-0.4</v>
       </c>
       <c r="D17">
         <v>3.2</v>
@@ -796,10 +796,10 @@
         <v>4</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>-1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-0.7</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -822,7 +822,7 @@
         <v>5.5</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>